<commit_message>
Update README to explain outputs/edited from 3.1 & 3.2 scripts
</commit_message>
<xml_diff>
--- a/data/raw/03.1b_edited-species-seeded2_corrected-seeded-in-mix_subplot.xlsx
+++ b/data/raw/03.1b_edited-species-seeded2_corrected-seeded-in-mix_subplot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:40009_{28A3A110-A06D-4DF3-ACB9-0ADAC0A6265D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A90705F-9890-495B-9BA2-76797B0FE745}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:40009_{28A3A110-A06D-4DF3-ACB9-0ADAC0A6265D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A7B0641-FD0A-49CB-9BC3-4BFCFFF62375}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -905,11 +905,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1044,9 +1043,42 @@
           <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Yellow highlighting indicates SpeciesSeeded value was changed. Usually descrepancies are because the PlotMix column is conflicting (species weren't included in both warm and cool mixes, so there can only be one for any of them per site).</a:t>
+            <a:t>Yellow highlighting indicates SpeciesSeeded value was changed. Usually </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>discrepancies</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> are because the PlotMix column is conflicting (species weren't included in both warm and cool mixes, so there can only be one for any of them per site).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1366,7 +1398,7 @@
   <dimension ref="A1:J166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
@@ -1461,7 +1493,7 @@
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">

</xml_diff>